<commit_message>
added some missing data and information
</commit_message>
<xml_diff>
--- a/data/raw/Data_ps_raw.xlsx
+++ b/data/raw/Data_ps_raw.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9a6394c8a17713bc/Research/Research projects/tDCS Motor Learning/tDCS_Motor_materials/data_thesis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9a6394c8a17713bc/Research/Research projects/tDCS meta-analysis/tDCS_meta-analysis/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="11_D795F8136DA38AC2F9D6B83D580132519B0F71F6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{75385A6F-CA45-45BC-97FD-A9D592453C2D}"/>
+  <xr:revisionPtr revIDLastSave="35" documentId="11_D795F8136DA38AC2F9D6B83D580132519B0F71F6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F9577FCA-8F40-4EC9-B2AF-A73DA303B501}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MA1" sheetId="1" r:id="rId1"/>
@@ -306,9 +306,6 @@
     <t>Eighteen chronic stroke patients participated in a randomized, crossover, placebo-controlled, double bind trial. During separate sessions, dual-tDCS or sham dual-tDCS was applied over 30 min while stroke patients learned a complex visuomotor skill with the paretic hand: using a computer mouse to move a pointer along a complex circuit as quickly and accurately as possible. A learning index involving the evolution of the speed/accuracy trade-off was calculated. Performance of the motor skill was measured at baseline, after intervention and 1 week later.</t>
   </si>
   <si>
-    <t xml:space="preserve">1st set of means and SDs is for 1st set of means and SDs is for baseline (control, from figure 3) and recall, 2nd set improvement from baseline. </t>
-  </si>
-  <si>
     <t>Lefebvre, Stéphanie; Dricot, Laurence; Laloux, Patrice; Gradkowski, Wojciech; Desfontaines, Philippe; Evrard, Frédéric; Peeters, André; Jamart, Jacques; Vandermeeren, Yves</t>
   </si>
   <si>
@@ -343,9 +340,6 @@
   </si>
   <si>
     <t>To investigate the combined effect of transcranial direct current stimulation (tDCS) and home-based occupational therapy on activities of daily living (ADL) and grip strength, in patients with upper limb motor impairment following intracerebral hemorrhage (ICH).</t>
-  </si>
-  <si>
-    <t>Means and SDs are for imrpovement from baseline</t>
   </si>
   <si>
     <t>Nair, Dinesh G.; Renga, Vijay; Lindenberg, Robert; Zhu, Lin; Schlaug, Gottfried</t>
@@ -644,9 +638,6 @@
     <t>UE-FM - Purpose: This pilot double-blind sham-controlled randomized trial aimed to determine if the addition of anodal tDCS on the affected hemisphere or cathodal tDCS on unaffected hemisphere to modified constraint-induced movement therapy (mCIMT) would be superior to constraints therapy alone in improving upper limb function in chronic stroke patients. Methods: Twenty-one patients with chronic stroke were randomly assigned to receive 12 sessions of either (i) anodal, (ii) cathodal or (iii) sham tDCS combined with mCIMT. Fugl–Meyer assessment (FMA), motor activity log scale (MAL), and handgrip strength were analyzed before, immediately, and 1 month (follow-up) after the treatment. Minimal clinically important difference (mCID) was defined as an increase of _x0002_5.25 in the upper limb FMA.</t>
   </si>
   <si>
-    <t>Tvalues from able 3</t>
-  </si>
-  <si>
     <t>Stagg, Charlotte Jane; Bachtiar, Velicia; O'Shea, Jacinta; Allman, Claire; Bosnell, Rosemary Ann; Kischka, Udo; Matthews, Paul McMahan; Johansen-Berg, Heidi</t>
   </si>
   <si>
@@ -831,6 +822,15 @@
   </si>
   <si>
     <t>Values (% changes) extracted from figure 2a</t>
+  </si>
+  <si>
+    <t>p. 4. Means and SDs are for percentage imrpovement from baseline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1st set of means and SDs is for baseline (control, from figure 3) and recall, 2nd set improvement from baseline. </t>
+  </si>
+  <si>
+    <t>values from able 3</t>
   </si>
 </sst>
 </file>
@@ -944,6 +944,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1150,10 +1154,10 @@
   <dimension ref="A1:AN1004"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="H5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D10" sqref="D10"/>
+      <selection pane="bottomRight" activeCell="R25" sqref="R25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1324,7 +1328,7 @@
       <c r="W2" s="1"/>
       <c r="X2" s="1"/>
       <c r="Y2" s="11" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="Z2" s="1"/>
       <c r="AA2" s="3">
@@ -1552,7 +1556,7 @@
       <c r="W5" s="1"/>
       <c r="X5" s="1"/>
       <c r="Y5" s="11" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="Z5" s="3" t="s">
         <v>60</v>
@@ -1858,7 +1862,7 @@
       <c r="W9" s="1"/>
       <c r="X9" s="1"/>
       <c r="Y9" s="11" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="Z9" s="3"/>
       <c r="AA9" s="3">
@@ -1934,7 +1938,7 @@
       <c r="W10" s="1"/>
       <c r="X10" s="1"/>
       <c r="Y10" s="11" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="Z10" s="3"/>
       <c r="AA10" s="3">
@@ -2010,7 +2014,7 @@
       <c r="W11" s="1"/>
       <c r="X11" s="1"/>
       <c r="Y11" s="11" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="Z11" s="3"/>
       <c r="AA11" s="3">
@@ -2086,7 +2090,7 @@
       <c r="W12" s="1"/>
       <c r="X12" s="1"/>
       <c r="Y12" s="11" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="Z12" s="3"/>
       <c r="AA12" s="3">
@@ -2174,7 +2178,7 @@
       <c r="W13" s="1"/>
       <c r="X13" s="1"/>
       <c r="Y13" s="11" t="s">
-        <v>90</v>
+        <v>260</v>
       </c>
       <c r="Z13" s="1"/>
       <c r="AA13" s="3">
@@ -2214,16 +2218,16 @@
         <v>13</v>
       </c>
       <c r="D14" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>92</v>
       </c>
       <c r="F14" s="3">
         <v>2015</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>45</v>
@@ -2262,13 +2266,13 @@
         <v>1.61</v>
       </c>
       <c r="W14" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="X14" s="1">
         <v>1</v>
       </c>
       <c r="Y14" s="11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="Z14" s="3"/>
       <c r="AA14" s="3">
@@ -2308,16 +2312,16 @@
         <v>14</v>
       </c>
       <c r="D15" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>97</v>
       </c>
       <c r="F15" s="3">
         <v>2010</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H15" s="3">
         <v>10</v>
@@ -2344,7 +2348,7 @@
       <c r="W15" s="1"/>
       <c r="X15" s="1"/>
       <c r="Y15" s="11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Z15" s="1"/>
       <c r="AA15" s="3">
@@ -2384,16 +2388,16 @@
         <v>15</v>
       </c>
       <c r="D16" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>100</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>101</v>
       </c>
       <c r="F16" s="3">
         <v>2016</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H16" s="3">
         <v>7</v>
@@ -2420,7 +2424,7 @@
       <c r="W16" s="1"/>
       <c r="X16" s="1"/>
       <c r="Y16" s="11" t="s">
-        <v>103</v>
+        <v>259</v>
       </c>
       <c r="Z16" s="3"/>
       <c r="AA16" s="3">
@@ -2460,16 +2464,16 @@
         <v>16</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F17" s="3">
         <v>2011</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="H17" s="3">
         <v>7</v>
@@ -2508,7 +2512,7 @@
       <c r="W17" s="1"/>
       <c r="X17" s="1"/>
       <c r="Y17" s="11" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="Z17" s="3"/>
       <c r="AA17" s="3">
@@ -2548,16 +2552,16 @@
         <v>17</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F18" s="3">
         <v>2016</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="H18" s="3">
         <v>7</v>
@@ -2624,16 +2628,16 @@
         <v>18</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F19" s="3">
         <v>2016</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H19" s="3">
         <v>7</v>
@@ -2700,16 +2704,16 @@
         <v>19</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F20" s="3">
         <v>2015</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="H20" s="3">
         <v>10</v>
@@ -2739,7 +2743,7 @@
       <c r="W20" s="1"/>
       <c r="X20" s="1"/>
       <c r="Y20" s="11" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="Z20" s="3"/>
       <c r="AA20" s="3">
@@ -2779,16 +2783,16 @@
         <v>20</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F21" s="3">
         <v>2013</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H21" s="3">
         <v>45</v>
@@ -2806,10 +2810,10 @@
         <v>1.430963459</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="N21" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="U21" s="2">
         <v>1E-3</v>
@@ -2818,7 +2822,7 @@
       <c r="W21" s="1"/>
       <c r="X21" s="1"/>
       <c r="Y21" s="11" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="Z21" s="1"/>
       <c r="AA21" s="3">
@@ -2858,16 +2862,16 @@
         <v>21</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F22" s="3">
         <v>2012</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>45</v>
@@ -2876,7 +2880,7 @@
         <v>45</v>
       </c>
       <c r="J22" s="3">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="K22" s="2">
         <v>56.1</v>
@@ -2889,12 +2893,24 @@
       </c>
       <c r="N22" s="1">
         <v>9.1</v>
+      </c>
+      <c r="O22">
+        <v>63.5</v>
+      </c>
+      <c r="P22">
+        <v>76.400000000000006</v>
+      </c>
+      <c r="Q22">
+        <v>9.1</v>
+      </c>
+      <c r="R22">
+        <v>9.1999999999999993</v>
       </c>
       <c r="V22" s="1"/>
       <c r="W22" s="1"/>
       <c r="X22" s="1"/>
       <c r="Y22" s="11" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="Z22" s="1"/>
       <c r="AA22" s="3">
@@ -9818,10 +9834,10 @@
   <dimension ref="A1:AR974"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="AB2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="AC2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AB23" sqref="AB23"/>
+      <selection pane="bottomRight" activeCell="AC24" sqref="AC24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -9886,16 +9902,16 @@
         <v>17</v>
       </c>
       <c r="S1" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="U1" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>127</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>129</v>
       </c>
       <c r="W1" s="2" t="s">
         <v>18</v>
@@ -9969,16 +9985,16 @@
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="F2" s="2">
         <v>2014</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>45</v>
@@ -10031,10 +10047,10 @@
       <c r="AA2" s="2"/>
       <c r="AB2" s="2"/>
       <c r="AC2" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="AD2" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="AE2" s="2">
         <v>10</v>
@@ -10062,7 +10078,7 @@
         <v>1.7</v>
       </c>
       <c r="AO2" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:44" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -10076,16 +10092,16 @@
         <v>2</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F3" s="2">
         <v>2007</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>45</v>
@@ -10114,10 +10130,10 @@
       <c r="AA3" s="2"/>
       <c r="AB3" s="2"/>
       <c r="AC3" s="7" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="AD3" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="AE3" s="2">
         <v>4</v>
@@ -10156,16 +10172,16 @@
         <v>3</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F4" s="2">
         <v>2017</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>45</v>
@@ -10183,16 +10199,16 @@
         <v>0.7</v>
       </c>
       <c r="AA4" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="AB4" s="2">
         <v>1</v>
       </c>
       <c r="AC4" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="AD4" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="AE4" s="2">
         <v>25</v>
@@ -10231,16 +10247,16 @@
         <v>4</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F5" s="2">
         <v>2005</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>45</v>
@@ -10278,10 +10294,10 @@
       <c r="AA5" s="2"/>
       <c r="AB5" s="2"/>
       <c r="AC5" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="AD5" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="AE5" s="2">
         <v>6</v>
@@ -10320,16 +10336,16 @@
         <v>5</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F6" s="2">
         <v>2013</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>45</v>
@@ -10373,10 +10389,10 @@
       <c r="AA6" s="2"/>
       <c r="AB6" s="2"/>
       <c r="AC6" s="8" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="AD6" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="AE6" s="2">
         <v>3</v>
@@ -10418,13 +10434,13 @@
         <v>55</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F7" s="2">
         <v>2014</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="H7" s="2">
         <v>6</v>
@@ -10454,10 +10470,10 @@
         <v>0.194817984</v>
       </c>
       <c r="Q7" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="R7" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="Y7" s="2">
         <v>0.92500000000000004</v>
@@ -10465,10 +10481,10 @@
       <c r="AA7" s="2"/>
       <c r="AB7" s="2"/>
       <c r="AC7" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="AD7" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="AE7" s="2">
         <v>6</v>
@@ -10510,13 +10526,13 @@
         <v>55</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F8" s="2">
         <v>2014</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="H8" s="2">
         <v>6</v>
@@ -10546,10 +10562,10 @@
         <v>33.785714290000001</v>
       </c>
       <c r="Q8" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="R8" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="Y8" s="2">
         <v>0.89700000000000002</v>
@@ -10557,10 +10573,10 @@
       <c r="AA8" s="2"/>
       <c r="AB8" s="2"/>
       <c r="AC8" s="4" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="AD8" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="AE8" s="2">
         <v>6</v>
@@ -10602,13 +10618,13 @@
         <v>65</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F9" s="2">
         <v>2011</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="H9" s="2">
         <v>32</v>
@@ -10631,10 +10647,10 @@
       <c r="AA9" s="2"/>
       <c r="AB9" s="2"/>
       <c r="AC9" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="AD9" s="9" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="AE9" s="2">
         <v>32</v>
@@ -10676,13 +10692,13 @@
         <v>65</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F10" s="2">
         <v>2011</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="H10" s="2">
         <v>32</v>
@@ -10711,10 +10727,10 @@
       <c r="AA10" s="2"/>
       <c r="AB10" s="2"/>
       <c r="AC10" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="AD10" s="9" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="AE10" s="2">
         <v>32</v>
@@ -10756,13 +10772,13 @@
         <v>71</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F11" s="2">
         <v>2013</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="H11" s="2">
         <v>13</v>
@@ -10780,18 +10796,18 @@
         <v>3.40010623</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="AA11" s="2"/>
       <c r="AB11" s="2"/>
       <c r="AC11" s="2" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="AD11" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="AE11" s="2">
         <v>13</v>
@@ -10833,13 +10849,13 @@
         <v>71</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F12" s="2">
         <v>2013</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="H12" s="2">
         <v>13</v>
@@ -10857,18 +10873,18 @@
         <v>6.9952203720000004</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="N12" s="2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="AA12" s="2"/>
       <c r="AB12" s="2"/>
       <c r="AC12" s="2" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="AD12" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="AE12" s="2">
         <v>13</v>
@@ -10910,13 +10926,13 @@
         <v>80</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F13" s="2">
         <v>2010</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="H13" s="2">
         <v>7</v>
@@ -10934,18 +10950,18 @@
         <v>52.925625369999999</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="N13" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="AA13" s="2"/>
       <c r="AB13" s="2"/>
       <c r="AC13" s="2" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="AD13" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="AE13" s="2">
         <v>7</v>
@@ -10984,16 +11000,16 @@
         <v>13</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F14" s="2">
         <v>2017</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>45</v>
@@ -11011,18 +11027,18 @@
         <v>-9.0438481379999995</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="N14" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="AA14" s="2"/>
       <c r="AB14" s="2"/>
       <c r="AC14" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="AD14" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="AE14" s="2">
         <v>25</v>
@@ -11061,16 +11077,16 @@
         <v>14</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F15" s="2">
         <v>2011</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="H15" s="2">
         <v>7</v>
@@ -11120,10 +11136,10 @@
       <c r="AA15" s="2"/>
       <c r="AB15" s="2"/>
       <c r="AC15" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="AD15" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="AE15" s="2">
         <v>7</v>
@@ -11162,16 +11178,16 @@
         <v>15</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F16" s="2">
         <v>2011</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="H16" s="2">
         <v>7</v>
@@ -11221,10 +11237,10 @@
       <c r="AA16" s="2"/>
       <c r="AB16" s="2"/>
       <c r="AC16" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="AD16" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="AE16" s="2">
         <v>7</v>
@@ -11263,16 +11279,16 @@
         <v>16</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F17" s="2">
         <v>2016</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="H17" s="2">
         <v>7</v>
@@ -11298,10 +11314,10 @@
       <c r="AA17" s="2"/>
       <c r="AB17" s="2"/>
       <c r="AC17" s="2" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="AD17" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="AE17" s="2">
         <v>7</v>
@@ -11340,16 +11356,16 @@
         <v>17</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F18" s="2">
         <v>2016</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="H18" s="2">
         <v>7</v>
@@ -11375,10 +11391,10 @@
       <c r="AA18" s="2"/>
       <c r="AB18" s="2"/>
       <c r="AC18" s="2" t="s">
-        <v>199</v>
+        <v>261</v>
       </c>
       <c r="AD18" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="AE18" s="2">
         <v>7</v>
@@ -11417,16 +11433,16 @@
         <v>18</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="F19" s="2">
         <v>2012</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>45</v>
@@ -11444,18 +11460,18 @@
         <v>-0.18575851400000001</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="N19" s="2" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="AA19" s="2"/>
       <c r="AB19" s="2"/>
       <c r="AC19" s="2" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="AD19" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="AE19" s="2">
         <v>13</v>
@@ -11494,16 +11510,16 @@
         <v>19</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="F20" s="2">
         <v>2015</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="H20" s="2" t="s">
         <v>45</v>
@@ -11520,10 +11536,10 @@
       <c r="AA20" s="2"/>
       <c r="AB20" s="2"/>
       <c r="AC20" s="2" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="AD20" s="2" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="AE20" s="2">
         <v>9</v>
@@ -11562,16 +11578,16 @@
         <v>20</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="F21" s="2">
         <v>2012</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="H21" s="2" t="s">
         <v>45</v>
@@ -11609,10 +11625,10 @@
       <c r="AA21" s="2"/>
       <c r="AB21" s="2"/>
       <c r="AC21" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="AD21" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="AE21" s="2">
         <v>12</v>
@@ -17358,10 +17374,10 @@
   <dimension ref="A1:AM966"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="Y2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J1" sqref="J1"/>
+      <selection pane="bottomRight" activeCell="AC6" sqref="AC6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -17493,16 +17509,16 @@
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="F2" s="2">
         <v>2020</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="H2" s="2">
         <v>20</v>
@@ -17519,10 +17535,10 @@
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
       <c r="Y2" s="9" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="Z2" s="2" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="AA2" s="2">
         <v>20</v>
@@ -17534,7 +17550,7 @@
         <v>0.84</v>
       </c>
       <c r="AE2" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="AF2" s="2">
         <v>1</v>
@@ -17560,16 +17576,16 @@
         <v>2</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="F3" s="2">
         <v>2020</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="H3" s="2">
         <v>20</v>
@@ -17608,10 +17624,10 @@
       <c r="T3" s="2"/>
       <c r="U3" s="2"/>
       <c r="Y3" s="9" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="Z3" s="2" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="AA3" s="2">
         <v>20</v>
@@ -17623,7 +17639,7 @@
         <v>0.251</v>
       </c>
       <c r="AE3" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="AF3" s="2">
         <v>1</v>
@@ -17649,16 +17665,16 @@
         <v>3</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="F4" s="2">
         <v>2020</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>45</v>
@@ -17675,10 +17691,10 @@
       <c r="W4" s="2"/>
       <c r="X4" s="2"/>
       <c r="Y4" s="9" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="Z4" s="2" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="AC4" s="2">
         <v>15</v>
@@ -17687,7 +17703,7 @@
         <v>0.98199999999999998</v>
       </c>
       <c r="AE4" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="AF4" s="2">
         <v>1</v>
@@ -17713,16 +17729,16 @@
         <v>4</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="F5" s="2">
         <v>2019</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="H5" s="2">
         <v>11</v>
@@ -17751,10 +17767,10 @@
       <c r="W5" s="2"/>
       <c r="X5" s="2"/>
       <c r="Y5" s="2" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="Z5" s="2" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="AA5" s="2">
         <v>11</v>
@@ -17766,7 +17782,7 @@
         <v>1.1919999999999999</v>
       </c>
       <c r="AE5" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="AF5" s="2">
         <v>1</v>
@@ -17792,16 +17808,16 @@
         <v>5</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="F6" s="2">
         <v>2018</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="H6" s="2">
         <v>19</v>
@@ -17842,10 +17858,10 @@
       <c r="W6" s="2"/>
       <c r="X6" s="2"/>
       <c r="Y6" s="2" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="Z6" s="2" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="AA6" s="2">
         <v>19</v>
@@ -17857,7 +17873,7 @@
         <v>0.58799999999999997</v>
       </c>
       <c r="AE6" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="AF6" s="2">
         <v>1</v>
@@ -17883,16 +17899,16 @@
         <v>6</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="F7" s="2">
         <v>2017</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="H7" s="2">
         <v>11</v>
@@ -17913,10 +17929,10 @@
       <c r="W7" s="2"/>
       <c r="X7" s="2"/>
       <c r="Y7" s="9" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="Z7" s="2" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="AA7" s="2">
         <v>11</v>
@@ -17928,7 +17944,7 @@
         <v>0.58499999999999996</v>
       </c>
       <c r="AE7" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="AF7" s="2">
         <v>1</v>
@@ -23723,13 +23739,13 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1" s="2" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -23768,7 +23784,7 @@
     </row>
     <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="B5" s="2">
         <f t="shared" ref="B5:C5" si="0">AVERAGE(B2:B4)</f>
@@ -23784,7 +23800,7 @@
     </row>
     <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="B6" s="2">
         <f t="shared" ref="B6:C6" si="1">STDEV(B2:B4)</f>
@@ -23805,7 +23821,7 @@
     </row>
     <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="D8" s="2">
         <f>AVERAGE(D2:D7)</f>
@@ -23814,7 +23830,7 @@
     </row>
     <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="D9" s="2">
         <f>STDEV(D2:D7)</f>
@@ -23823,10 +23839,10 @@
     </row>
     <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="2" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
   </sheetData>

</xml_diff>